<commit_message>
edits to corinne's data
</commit_message>
<xml_diff>
--- a/step length and nsd calculations.xlsx
+++ b/step length and nsd calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Kane\Documents\Manuscripts\vulture_habitat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82712952-BA20-46B5-B89C-935B6A8B5935}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6321BBFF-4126-4316-BDE9-3DAF33327A27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27420" yWindow="3285" windowWidth="11835" windowHeight="15435" xr2:uid="{EA09CCF0-30A6-4983-B867-52D18F5F0E6D}"/>
+    <workbookView xWindow="17295" yWindow="5310" windowWidth="17340" windowHeight="15435" xr2:uid="{EA09CCF0-30A6-4983-B867-52D18F5F0E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,6 @@
     <t>nsd</t>
   </si>
   <si>
-    <t>CK151400_x</t>
-  </si>
-  <si>
-    <t>CK151400_y</t>
-  </si>
-  <si>
     <t>https://cran.r-project.org/web/packages/amt/vignettes/p1_getting_started.html</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>formula step length</t>
+  </si>
+  <si>
+    <t>#109018542 x_</t>
+  </si>
+  <si>
+    <t>#109018542 y_</t>
   </si>
 </sst>
 </file>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E64FF09-81A6-4D7D-B871-0E06E7627755}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,10 +490,10 @@
         <v>4</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -559,7 +559,7 @@
         <v>1269.7117783182134</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -585,27 +585,27 @@
         <v>1612168</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>

</xml_diff>